<commit_message>
FIX: Planificación terminada y ServletProductos arreglado
</commit_message>
<xml_diff>
--- a/planificacionSustitos.xlsx
+++ b/planificacionSustitos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC41E6A5-02A2-428F-9223-C9B914E74AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE46947-FF08-429E-A62E-DF6E05BE43DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>FECHA INICIO</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Jon</t>
   </si>
   <si>
-    <t>Finalizacion de la planificacion</t>
-  </si>
-  <si>
     <t>Omar</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Creacion de la vista y servlets de listado productos | FUNCIONALIDADES : Listar productos</t>
   </si>
   <si>
-    <t>Creacion de la vista de perfil de usuario y detalle productos, ademas de sus servlets | FUNCIONALIDADES : Mostrar detalles de productos y cambiar el usuario</t>
-  </si>
-  <si>
     <t>Creacion de la vista y servlets de detalle proveedores | FUNCIONALIDADES : Mostrar los detalles del los proveedores</t>
   </si>
   <si>
@@ -108,17 +102,95 @@
     <t>Creacion de la vista y servlets  validador | FUNCIONALIDADES : Enviar el correo y verificar</t>
   </si>
   <si>
-    <t>Jon, Omar, Chej</t>
-  </si>
-  <si>
     <t>Correccion de todos los errores que puedan pasar</t>
+  </si>
+  <si>
+    <t>Omar, Chej</t>
+  </si>
+  <si>
+    <t>Creacion de la vista y servlets de recuperar contraseña | FUNCIONALIDADES : Enviar correo al usuario para restablecer la contraseña</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>Sin problemas</t>
+  </si>
+  <si>
+    <t>No he podido sacar el tema del email ya que me estaba llevando más del tiempo establecido</t>
+  </si>
+  <si>
+    <t>Al final he tenido problemas al montar la base de datos que al final he solucionado y me ha lleva 4 horas en total</t>
+  </si>
+  <si>
+    <t>A medida que hemos ido avanzando hemos tenido que añair nuevas pantallas, por lo que ha supuesto un tiempo extra que no hemos podido calcular</t>
+  </si>
+  <si>
+    <t>La función para validar cuentas mediante el email esta hecha pero no cumple con su función por lo que no se puede validar al usuario mediante el email.  NOTA: Para validar a los usuarios hay que introducir "AAAA"</t>
+  </si>
+  <si>
+    <t>Modificación vista login  | UPDATE: Formulario para validar al usuario que se acaba de registrar</t>
+  </si>
+  <si>
+    <t>Si queremos modificar algun proveedor lo hace correctamente pero no modifica el fichero por tema de rutas; no se ha podido solucionar y nos ha llevado muchas horas extra</t>
+  </si>
+  <si>
+    <t>Hay una pantalla para usuarios y otra para admins. La de usuarios se ha completado sin problemas pero la de admin queda añadir un producto nuevo</t>
+  </si>
+  <si>
+    <t>Creacion de la vista de perfil de usuarios, ademas de su servlets | FUNCIONALIDADES : Mostrar detalles de cada usuario</t>
+  </si>
+  <si>
+    <t>Creacion de la vista detalle productos, ademas de sus servlets | FUNCIONALIDADES : Mostrar detalles de productos</t>
+  </si>
+  <si>
+    <t>La vista esta terminada pero queda por hacer que muestre los datos de ese usuario.</t>
+  </si>
+  <si>
+    <t>No manda el correo al usuario pero, anteriormente informe de que la cadena para validar usuarios es "AAAA"</t>
+  </si>
+  <si>
+    <t>No ha dado tiempo por problemas que han ido surgiendo</t>
+  </si>
+  <si>
+    <t>No se ha llegado a una solución clara</t>
+  </si>
+  <si>
+    <t>Lo comentado anteriormente en este apartado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El metodo para validar el email no funciona </t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>30/02/2023</t>
+  </si>
+  <si>
+    <t>Creacion del pool de conexiones | FUNCIONALIDADES: Establecer conexión con la base de datos</t>
+  </si>
+  <si>
+    <t>Algunos errores no se han podido arreglar por la escasez del tiempo pero otros como el error que daba al entrar por primera vez en la vista listadoProducto.jsp esta arreglado.</t>
+  </si>
+  <si>
+    <t>TERMINADO</t>
+  </si>
+  <si>
+    <t>TERMINADO CON PROBLEMAS</t>
+  </si>
+  <si>
+    <t>Hemos tenido que crear otra vista para admins con información diferente.</t>
+  </si>
+  <si>
+    <t>SIN EMPEZAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.34998626667073579"/>
@@ -156,8 +228,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +246,24 @@
       <patternFill patternType="lightUp">
         <fgColor theme="0" tint="-0.14993743705557422"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,7 +288,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -223,6 +319,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -230,7 +335,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="3" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="3" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="3" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -255,9 +375,6 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="3" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -312,11 +429,11 @@
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleLight2">
     <tableStyle name="Análisis de la competencia" pivot="0" count="5" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
-      <tableStyleElement type="firstColumn" dxfId="10"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstColumn" dxfId="14"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -331,13 +448,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Análisis" displayName="Análisis" ref="B3:F7" totalsRowShown="0">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PARTICIPANTES" totalsRowDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="FECHA INICIO" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="FECHA FIN" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="HORAS" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="TAREA" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Análisis" displayName="Análisis" ref="B3:H10" totalsRowShown="0">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PARTICIPANTES" totalsRowDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="FECHA INICIO" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="FECHA FIN" dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="HORAS" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="TAREA" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F415E5DD-FA62-4EFB-A595-C13A17312205}" name="COMENTARIOS" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{DBEB5C9E-FDEC-46E0-B601-D748C6859C58}" name="ESTADO" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Análisis de la competencia" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -614,10 +733,10 @@
     <tabColor theme="1" tint="0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F22"/>
+  <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,10 +747,12 @@
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="97.140625" customWidth="1"/>
+    <col min="7" max="7" width="54.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -640,7 +761,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
@@ -656,8 +777,14 @@
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -673,8 +800,14 @@
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -685,13 +818,19 @@
         <v>44956</v>
       </c>
       <c r="E5" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -702,64 +841,88 @@
         <v>44956</v>
       </c>
       <c r="E6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44960</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="6">
         <v>44956</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="6">
         <v>44929</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="G8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="6">
-        <v>44958</v>
-      </c>
-      <c r="D8" s="6">
-        <v>44958</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1.45</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="C9" s="6">
         <v>44958</v>
       </c>
       <c r="D9" s="6">
-        <v>44960</v>
+        <v>44958</v>
       </c>
       <c r="E9" s="7">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -770,15 +933,21 @@
         <v>44958</v>
       </c>
       <c r="E10" s="7">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" s="6">
         <v>44958</v>
@@ -787,201 +956,343 @@
         <v>44958</v>
       </c>
       <c r="E11" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6">
         <v>44958</v>
       </c>
       <c r="D12" s="6">
-        <v>44958</v>
+        <v>44960</v>
       </c>
       <c r="E12" s="7">
         <v>3</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6">
+        <v>44958</v>
+      </c>
+      <c r="D13" s="6">
         <v>44960</v>
       </c>
-      <c r="D13" s="6">
-        <v>44963</v>
-      </c>
       <c r="E13" s="7">
-        <v>4</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C14" s="6">
         <v>44960</v>
       </c>
       <c r="D14" s="6">
-        <v>44963</v>
+        <v>44962</v>
       </c>
       <c r="E14" s="7">
-        <v>4</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C15" s="6">
         <v>44960</v>
       </c>
       <c r="D15" s="6">
-        <v>44963</v>
+        <v>44962</v>
       </c>
       <c r="E15" s="7">
-        <v>4</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="6">
-        <v>44964</v>
+        <v>44960</v>
       </c>
       <c r="D16" s="6">
-        <v>44965</v>
+        <v>44962</v>
       </c>
       <c r="E16" s="7">
         <v>4</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6">
+        <v>44962</v>
+      </c>
+      <c r="D17" s="6">
         <v>44964</v>
-      </c>
-      <c r="D17" s="6">
-        <v>44965</v>
       </c>
       <c r="E17" s="7">
         <v>4</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="6">
+        <v>44962</v>
+      </c>
+      <c r="D18" s="6">
         <v>44964</v>
-      </c>
-      <c r="D18" s="6">
-        <v>44965</v>
       </c>
       <c r="E18" s="7">
         <v>4</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6">
+        <v>44962</v>
+      </c>
+      <c r="D19" s="6">
+        <v>44964</v>
+      </c>
+      <c r="E19" s="7">
+        <v>4</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="6">
+        <v>44964</v>
+      </c>
+      <c r="D20" s="6">
         <v>44965</v>
       </c>
-      <c r="D19" s="6">
+      <c r="E20" s="7">
+        <v>4</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6">
+        <v>44964</v>
+      </c>
+      <c r="D21" s="6">
+        <v>44965</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6">
+        <v>44964</v>
+      </c>
+      <c r="D22" s="6">
+        <v>44965</v>
+      </c>
+      <c r="E22" s="7">
+        <v>3</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6">
+        <v>44964</v>
+      </c>
+      <c r="D23" s="6">
+        <v>44966</v>
+      </c>
+      <c r="E23" s="7">
+        <v>4</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="6">
+        <v>44965</v>
+      </c>
+      <c r="D24" s="6">
         <v>44967</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E24" s="7">
         <v>3</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="6">
+        <v>44967</v>
+      </c>
+      <c r="D25" s="6">
+        <v>44967</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="6">
-        <v>44965</v>
-      </c>
-      <c r="D20" s="6">
-        <v>44967</v>
-      </c>
-      <c r="E20" s="7">
-        <v>3</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="6">
-        <v>44965</v>
-      </c>
-      <c r="D21" s="6">
-        <v>44967</v>
-      </c>
-      <c r="E21" s="7">
-        <v>3</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="6">
-        <v>44967</v>
-      </c>
-      <c r="D22" s="6">
-        <v>44967</v>
-      </c>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>30</v>
+      <c r="G25" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la información en la tabla Análisis que comienza en la celda B5 en esta hoja de cálculo. Seleccione la celda B3 para volver a la hoja de cálculo Datos demográficos de los competidores." sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El título de esta hoja de cálculo se encuentra en esta celda. El nombre de la empresa se actualiza automáticamente en función de la entrada en la celda B2 de la hoja de cálculo Datos demográficos de los competidores." sqref="B2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
@@ -989,8 +1300,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use la leyenda de la fila 4 para calificar los establecimientos minoristas en una escala de 0 a 4 en esta columna, debajo de este encabezado." sqref="C3" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use la leyenda de la fila 4 para calificar las ventas anuales en una escala de 0 a 4 en esta columna, debajo de este encabezado." sqref="D3" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use la leyenda de la fila 4 para calificar la comparación de productos en una escala de 0 a 4 en esta columna, debajo de este encabezado." sqref="E3" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use la leyenda de la fila 4 para calificar el precio de los productos en una escala de 0 a 4 en esta columna, debajo de este encabezado." sqref="F3" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione una opción de la lista. Seleccione CANCELAR, presione ALT+FLECHA ABAJO para ver las opciones y, después, use la tecla de FLECHA ABAJO y ENTRAR para realizar una selección." sqref="B4:B10" xr:uid="{00000000-0002-0000-0100-000012000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use la leyenda de la fila 4 para calificar el precio de los productos en una escala de 0 a 4 en esta columna, debajo de este encabezado." sqref="F3:H3" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Seleccione una opción de la lista. Seleccione CANCELAR, presione ALT+FLECHA ABAJO para ver las opciones y, después, use la tecla de FLECHA ABAJO y ENTRAR para realizar una selección." sqref="B4:B6 B8:B14" xr:uid="{00000000-0002-0000-0100-000012000000}">
       <formula1>Competidores</formula1>
     </dataValidation>
   </dataValidations>
@@ -1007,15 +1318,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1303,6 +1605,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1324,14 +1635,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF49CB3-19D5-457E-B30F-E542C450FC26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393B498D-0CA7-4201-9223-2C008CB80913}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1352,6 +1655,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF49CB3-19D5-457E-B30F-E542C450FC26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{777A5722-4D33-44FE-9814-D64063D0A4E5}">
   <ds:schemaRefs>

</xml_diff>